<commit_message>
Add histomorphometric quantification scripts
- Alpl coverage quantification
- Statistical analysis
- TRAP and Ctsk positivity
</commit_message>
<xml_diff>
--- a/raw-data/Bmp7-CT-scans.xlsx
+++ b/raw-data/Bmp7-CT-scans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmrot\Documents\R\Bmp7-ins\raw-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C06A743-67CC-42C7-A88C-6D001DA09187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C171337-A723-4E6C-8972-B1156AF7FDDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="13824" windowHeight="7104" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1057,9 +1057,9 @@
   </sheetPr>
   <dimension ref="A1:AC965"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AB63" sqref="AB63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1462,7 +1462,10 @@
         <v>27</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
@@ -1756,7 +1759,10 @@
         <v>44510</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -1776,7 +1782,10 @@
         <v>44510</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -1816,7 +1825,10 @@
         <v>43675</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">

</xml_diff>